<commit_message>
optimized regression run code, return time
</commit_message>
<xml_diff>
--- a/FSX_QA_SERVICE/edp_regression_test/report/edp_report.xlsx
+++ b/FSX_QA_SERVICE/edp_regression_test/report/edp_report.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,16 +575,8 @@
         </is>
       </c>
       <c r="I2" s="5" t="n"/>
-      <c r="J2" s="5" t="inlineStr">
-        <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010013,No available instrument risk check data found: instrumentDate=not_found,expectedDate=20230913</t>
-        </is>
-      </c>
+      <c r="J2" s="5" t="n"/>
+      <c r="K2" s="5" t="n"/>
       <c r="L2" s="5" t="n"/>
       <c r="M2" s="5" t="inlineStr">
         <is>
@@ -592,29 +584,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>ERROR_10010013,No available instrument risk check data found: instrumentDate=not_found,expectedDate=20230913</t>
-        </is>
-      </c>
-    </row>
     <row r="4">
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>ERROR_10010013,No available instrument risk check data found: instrumentDate=not_found,expectedDate=20230913</t>
-        </is>
-      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>FixMsg is OK</t>
@@ -622,31 +592,9 @@
       </c>
     </row>
     <row r="5">
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>ERROR_10010013,No available instrument risk check data found: instrumentDate=not_found,expectedDate=20230913</t>
-        </is>
-      </c>
       <c r="M5" t="inlineStr">
         <is>
           <t>execType is OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>ERROR_10010013,No available instrument risk check data found: instrumentDate=not_found,expectedDate=20230913</t>
         </is>
       </c>
     </row>

</xml_diff>